<commit_message>
works for one subscriptions and a first stab at SubscriptionManager doc changes
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B178DBF0-B915-4809-81FC-4BBF724732B9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB466B9-4674-4881-802F-A4D4713DF36B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ETHUSDT</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>BTCUSDT</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -166,18 +172,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -195,7 +208,7 @@
   <volType type="realTimeData">
     <main first="rabbit">
       <tp>
-        <v>585.21</v>
+        <v>579.59</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -204,7 +217,7 @@
         <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>585.44000000000005</v>
+        <v>579.96</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -213,7 +226,25 @@
         <tr r="D4" s="1"/>
       </tp>
       <tp>
-        <v>585.32500000000005</v>
+        <v>1527208654949</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>BTCUSDT</stp>
+        <stp>O</stp>
+        <tr r="E4" s="1"/>
+      </tp>
+      <tp>
+        <v>1527295054641</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHUSDT</stp>
+        <stp>t</stp>
+        <tr r="G9" s="1"/>
+      </tp>
+      <tp>
+        <v>579.77499999999998</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -222,7 +253,7 @@
         <tr r="F9" s="1"/>
       </tp>
       <tp>
-        <v>585.44000000000005</v>
+        <v>579.96</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -231,7 +262,7 @@
         <tr r="D3" s="1"/>
       </tp>
       <tp>
-        <v>585.21</v>
+        <v>579.59</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -240,7 +271,25 @@
         <tr r="C3" s="1"/>
       </tp>
       <tp>
-        <v>585.32500000000005</v>
+        <v>1527208654949</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ETHUSDT</stp>
+        <stp>O</stp>
+        <tr r="E3" s="1"/>
+      </tp>
+      <tp>
+        <v>1527295054641</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BTCUSDT</stp>
+        <stp>t</stp>
+        <tr r="G10" s="1"/>
+      </tp>
+      <tp>
+        <v>579.77499999999998</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -254,15 +303,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:D4" totalsRowShown="0">
-  <autoFilter ref="B2:D4" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:E4" totalsRowShown="0">
+  <autoFilter ref="B2:E4" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4684B3D0-E19D-45C0-AF8D-58548797FDAF}" name="Symbol"/>
     <tableColumn id="2" xr3:uid="{025AE9D2-02E3-4A4E-9988-5BB682835FAE}" name="b">
       <calculatedColumnFormula>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{ECCD1A0A-D497-4C73-BD19-851157FDDFA6}" name="a">
       <calculatedColumnFormula>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{04F17769-55A0-4978-9AF0-73C1BFD079FB}" name="O" dataDxfId="0">
+      <calculatedColumnFormula>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -566,17 +618,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35C332D-6131-427D-B374-A8266C368C7A}">
-  <dimension ref="B1:H10"/>
+  <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -594,6 +648,9 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -601,11 +658,15 @@
       </c>
       <c r="C3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>585.21</v>
+        <v>579.59</v>
       </c>
       <c r="D3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>585.44000000000005</v>
+        <v>579.96</v>
+      </c>
+      <c r="E3" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
+        <v>1527208654949</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -614,11 +675,15 @@
       </c>
       <c r="C4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>585.21</v>
+        <v>579.59</v>
       </c>
       <c r="D4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>585.44000000000005</v>
+        <v>579.96</v>
+      </c>
+      <c r="E4" s="7">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
+        <v>1527208654949</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -641,6 +706,9 @@
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
       <c r="H8" t="s">
         <v>8</v>
       </c>
@@ -648,7 +716,11 @@
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F9" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,F$8)</f>
-        <v>585.32500000000005</v>
+        <v>579.77499999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,G$8)</f>
+        <v>1527295054641</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
@@ -657,16 +729,24 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F10" s="4">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,F$8)</f>
-        <v>585.32500000000005</v>
+        <v>579.77499999999998</v>
+      </c>
+      <c r="G10" s="6">
+        <f>RTD("rabbit",,"localhost","MODEL",$B4,G$8)</f>
+        <v>1527295054641</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
two streams seperated by routingKey
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB466B9-4674-4881-802F-A4D4713DF36B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB60BB3-4A7A-45D1-94A4-3B265AF88378}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
@@ -27,52 +27,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>BINANCE</t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>This data come from Rabbit MQ</t>
+  </si>
+  <si>
+    <t>Model Listens to RabbitMQ</t>
+  </si>
+  <si>
+    <t>Calculating Mid Price</t>
+  </si>
+  <si>
+    <t>Publishing back on RabbitMQ</t>
+  </si>
+  <si>
+    <t>Get Delivered to Model</t>
+  </si>
+  <si>
+    <t>And to this Spreadsheet</t>
+  </si>
+  <si>
+    <t>BTCUSDT</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>ETHUSDT</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>BINANCE</t>
-  </si>
-  <si>
-    <t>MODEL</t>
-  </si>
-  <si>
-    <t>This data come from Rabbit MQ</t>
-  </si>
-  <si>
-    <t>Model Listens to RabbitMQ</t>
-  </si>
-  <si>
-    <t>Calculating Mid Price</t>
-  </si>
-  <si>
-    <t>Publishing back on RabbitMQ</t>
-  </si>
-  <si>
-    <t>Get Delivered to Model</t>
-  </si>
-  <si>
-    <t>And to this Spreadsheet</t>
-  </si>
-  <si>
-    <t>BTCUSDT</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>O</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
   <volType type="realTimeData">
     <main first="rabbit">
       <tp>
-        <v>579.59</v>
+        <v>7536.4</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -217,7 +217,7 @@
         <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>579.96</v>
+        <v>7542.23</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -226,7 +226,7 @@
         <tr r="D4" s="1"/>
       </tp>
       <tp>
-        <v>1527208654949</v>
+        <v>1527256924701</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -234,8 +234,8 @@
         <stp>O</stp>
         <tr r="E4" s="1"/>
       </tp>
-      <tp>
-        <v>1527295054641</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -243,8 +243,8 @@
         <stp>t</stp>
         <tr r="G9" s="1"/>
       </tp>
-      <tp>
-        <v>579.77499999999998</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -252,8 +252,8 @@
         <stp>m</stp>
         <tr r="F9" s="1"/>
       </tp>
-      <tp>
-        <v>579.96</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -261,8 +261,8 @@
         <stp>a</stp>
         <tr r="D3" s="1"/>
       </tp>
-      <tp>
-        <v>579.59</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -270,8 +270,8 @@
         <stp>b</stp>
         <tr r="C3" s="1"/>
       </tp>
-      <tp>
-        <v>1527208654949</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -279,8 +279,8 @@
         <stp>O</stp>
         <tr r="E3" s="1"/>
       </tp>
-      <tp>
-        <v>1527295054641</v>
+      <tp t="s">
+        <v>0001-01-01T00:00:00</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -289,7 +289,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>579.77499999999998</v>
+        <v>603.76</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -621,7 +621,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,108 +635,108 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>579.59</v>
-      </c>
-      <c r="D3">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D3" t="str">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>579.96</v>
-      </c>
-      <c r="E3" s="5">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="E3" s="5" t="str">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
-        <v>1527208654949</v>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>579.59</v>
+        <v>7536.4</v>
       </c>
       <c r="D4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>579.96</v>
+        <v>7542.23</v>
       </c>
       <c r="E4" s="7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
-        <v>1527208654949</v>
+        <v>1527256924701</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="3" t="str">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,F$8)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G9" s="6" t="str">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,G$8)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H9" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="3">
-        <f>RTD("rabbit",,"localhost","MODEL",$B3,F$8)</f>
-        <v>579.77499999999998</v>
-      </c>
-      <c r="G9" s="6">
-        <f>RTD("rabbit",,"localhost","MODEL",$B3,G$8)</f>
-        <v>1527295054641</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F10" s="4">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,F$8)</f>
-        <v>579.77499999999998</v>
-      </c>
-      <c r="G10" s="6">
+        <v>603.76</v>
+      </c>
+      <c r="G10" s="6" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,G$8)</f>
-        <v>1527295054641</v>
+        <v>0001-01-01T00:00:00</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
trying to display unix timestamps
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB60BB3-4A7A-45D1-94A4-3B265AF88378}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C318E4C6-6A90-4DBB-9A0B-209A142FD1F5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Symbol</t>
   </si>
@@ -45,24 +45,12 @@
     <t>MODEL</t>
   </si>
   <si>
-    <t>This data come from Rabbit MQ</t>
-  </si>
-  <si>
     <t>Model Listens to RabbitMQ</t>
   </si>
   <si>
     <t>Calculating Mid Price</t>
   </si>
   <si>
-    <t>Publishing back on RabbitMQ</t>
-  </si>
-  <si>
-    <t>Get Delivered to Model</t>
-  </si>
-  <si>
-    <t>And to this Spreadsheet</t>
-  </si>
-  <si>
     <t>BTCUSDT</t>
   </si>
   <si>
@@ -73,15 +61,36 @@
   </si>
   <si>
     <t>ETHUSDT</t>
+  </si>
+  <si>
+    <t>LTCUSDT</t>
+  </si>
+  <si>
+    <t>ZENBTC</t>
+  </si>
+  <si>
+    <t>ETHBTC</t>
+  </si>
+  <si>
+    <t>LTCBTC</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>BINANCE_AGGR_TRADE</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,20 +176,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -188,7 +206,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -207,95 +225,437 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="rabbit">
-      <tp>
-        <v>7536.4</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>LTCBTC</stp>
+        <stp>q</stp>
+        <tr r="J8" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>LTCBTC</stp>
+        <stp>p</stp>
+        <tr r="I8" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ETHBTC</stp>
+        <stp>q</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ETHBTC</stp>
+        <stp>p</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp>
+        <v>118.01</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>p</stp>
+        <tr r="I5" s="1"/>
+      </tp>
+      <tp>
+        <v>0.5</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>q</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+      <tp>
+        <v>7310</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>BTCUSDT</stp>
+        <stp>p</stp>
+        <tr r="I3" s="1"/>
+      </tp>
+      <tp>
+        <v>5.5120000000000004E-3</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>BTCUSDT</stp>
+        <stp>q</stp>
+        <tr r="J3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ZENBTC</stp>
+        <stp>q</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ZENBTC</stp>
+        <stp>p</stp>
+        <tr r="I6" s="1"/>
+      </tp>
+      <tp>
+        <v>7.0989999999999998E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ETHUSDT</stp>
+        <stp>q</stp>
+        <tr r="J4" s="1"/>
+      </tp>
+      <tp>
+        <v>567.70000000000005</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ETHUSDT</stp>
+        <stp>p</stp>
+        <tr r="I4" s="1"/>
+      </tp>
+      <tp>
+        <v>-2310</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>t</stp>
+        <tr r="H7" s="1"/>
+      </tp>
+      <tp>
+        <v>7.7629500000000004E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>m</stp>
+        <tr r="F7" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036366</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>C</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp>
+        <v>-2139</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>t</stp>
+        <tr r="H8" s="1"/>
+      </tp>
+      <tp>
+        <v>1.61485E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>m</stp>
+        <tr r="F8" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036195</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>C</stp>
+        <tr r="G8" s="1"/>
+      </tp>
+      <tp>
+        <v>-2133</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>t</stp>
+        <tr r="H6" s="1"/>
+      </tp>
+      <tp>
+        <v>4.5189999999999996E-3</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>m</stp>
+        <tr r="F6" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036247</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>C</stp>
+        <tr r="G6" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636195</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCBTC</stp>
+        <stp>O</stp>
+        <tr r="E8" s="1"/>
+      </tp>
+      <tp>
+        <v>1.6163E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCBTC</stp>
+        <stp>a</stp>
+        <tr r="D8" s="1"/>
+      </tp>
+      <tp>
+        <v>1.6133999999999999E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCBTC</stp>
+        <stp>b</stp>
+        <tr r="C8" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636366</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ETHBTC</stp>
+        <stp>O</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp>
+        <v>7.7644000000000005E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ETHBTC</stp>
+        <stp>a</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp>
+        <v>7.7615000000000003E-2</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ETHBTC</stp>
+        <stp>b</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+      <tp>
+        <v>7300.26</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>BTCUSDT</stp>
         <stp>b</stp>
-        <tr r="C4" s="1"/>
-      </tp>
-      <tp>
-        <v>7542.23</v>
+        <tr r="C3" s="1"/>
+      </tp>
+      <tp>
+        <v>7311.66</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>BTCUSDT</stp>
         <stp>a</stp>
-        <tr r="D4" s="1"/>
-      </tp>
-      <tp>
-        <v>1527256924701</v>
+        <tr r="D3" s="1"/>
+      </tp>
+      <tp>
+        <v>118.19</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>a</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+      <tp>
+        <v>117.9</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>b</stp>
+        <tr r="C5" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636327</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>O</stp>
+        <tr r="E5" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636374</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>BTCUSDT</stp>
         <stp>O</stp>
-        <tr r="E4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+        <tr r="E3" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636247</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ZENBTC</stp>
+        <stp>O</stp>
+        <tr r="E6" s="1"/>
+      </tp>
+      <tp>
+        <v>4.529E-3</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ZENBTC</stp>
+        <stp>a</stp>
+        <tr r="D6" s="1"/>
+      </tp>
+      <tp>
+        <v>4.509E-3</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>ZENBTC</stp>
+        <stp>b</stp>
+        <tr r="C6" s="1"/>
+      </tp>
+      <tp>
+        <v>-2279</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>ETHUSDT</stp>
         <stp>t</stp>
-        <tr r="G9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+        <tr r="H4" s="1"/>
+      </tp>
+      <tp>
+        <v>567.40499999999997</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>ETHUSDT</stp>
         <stp>m</stp>
-        <tr r="F9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+        <tr r="F4" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036336</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHUSDT</stp>
+        <stp>C</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+      <tp>
+        <v>567.73</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ETHUSDT</stp>
         <stp>a</stp>
-        <tr r="D3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+        <tr r="D4" s="1"/>
+      </tp>
+      <tp>
+        <v>567.08000000000004</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ETHUSDT</stp>
         <stp>b</stp>
-        <tr r="C3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+        <tr r="C4" s="1"/>
+      </tp>
+      <tp>
+        <v>1527358636336</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ETHUSDT</stp>
         <stp>O</stp>
-        <tr r="E3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>0001-01-01T00:00:00</v>
+        <tr r="E4" s="1"/>
+      </tp>
+      <tp>
+        <v>-2236</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>t</stp>
+        <tr r="H5" s="1"/>
+      </tp>
+      <tp>
+        <v>-2317</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>BTCUSDT</stp>
         <stp>t</stp>
-        <tr r="G10" s="1"/>
-      </tp>
-      <tp>
-        <v>603.76</v>
+        <tr r="H3" s="1"/>
+      </tp>
+      <tp>
+        <v>7305.96</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>BTCUSDT</stp>
         <stp>m</stp>
-        <tr r="F10" s="1"/>
+        <tr r="F3" s="1"/>
+      </tp>
+      <tp>
+        <v>118.045</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>m</stp>
+        <tr r="F5" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036327</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>C</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+      <tp>
+        <v>1527445036374</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BTCUSDT</stp>
+        <stp>C</stp>
+        <tr r="G3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -303,8 +663,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:E4" totalsRowShown="0">
-  <autoFilter ref="B2:E4" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:E8" totalsRowShown="0">
+  <autoFilter ref="B2:E8" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4684B3D0-E19D-45C0-AF8D-58548797FDAF}" name="Symbol"/>
     <tableColumn id="2" xr3:uid="{025AE9D2-02E3-4A4E-9988-5BB682835FAE}" name="b">
@@ -618,27 +978,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35C332D-6131-427D-B374-A8266C368C7A}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -649,98 +1016,251 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="str">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="D3" t="str">
+        <v>7300.26</v>
+      </c>
+      <c r="D3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="E3" s="5" t="str">
+        <v>7311.66</v>
+      </c>
+      <c r="E3" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
-        <v>&lt;?&gt;</v>
+        <v>1527358636374</v>
+      </c>
+      <c r="F3" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,F$2)</f>
+        <v>7305.96</v>
+      </c>
+      <c r="G3" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,G$2)</f>
+        <v>1527445036374</v>
+      </c>
+      <c r="H3" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B3,H$2)</f>
+        <v>-2317</v>
+      </c>
+      <c r="I3" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B3,I$2)</f>
+        <v>7310</v>
+      </c>
+      <c r="J3" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B3,J$2)</f>
+        <v>5.5120000000000004E-3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>7536.4</v>
+        <v>567.08000000000004</v>
       </c>
       <c r="D4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>7542.23</v>
-      </c>
-      <c r="E4" s="7">
+        <v>567.73</v>
+      </c>
+      <c r="E4" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
-        <v>1527256924701</v>
+        <v>1527358636336</v>
+      </c>
+      <c r="F4" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B4,F$2)</f>
+        <v>567.40499999999997</v>
+      </c>
+      <c r="G4" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B4,G$2)</f>
+        <v>1527445036336</v>
+      </c>
+      <c r="H4" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B4,H$2)</f>
+        <v>-2279</v>
+      </c>
+      <c r="I4" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B4,I$2)</f>
+        <v>567.70000000000005</v>
+      </c>
+      <c r="J4" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B4,J$2)</f>
+        <v>7.0989999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B5,C$2)</f>
+        <v>117.9</v>
+      </c>
+      <c r="D5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B5,D$2)</f>
+        <v>118.19</v>
+      </c>
+      <c r="E5" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B5,E$2)</f>
+        <v>1527358636327</v>
+      </c>
+      <c r="F5" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B5,F$2)</f>
+        <v>118.045</v>
+      </c>
+      <c r="G5" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B5,G$2)</f>
+        <v>1527445036327</v>
+      </c>
+      <c r="H5" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B5,H$2)</f>
+        <v>-2236</v>
+      </c>
+      <c r="I5" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B5,I$2)</f>
+        <v>118.01</v>
+      </c>
+      <c r="J5" s="4">
+        <f>RTD("rabbit",,"localhost",$I$1,$B5,J$2)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B6,C$2)</f>
+        <v>4.509E-3</v>
+      </c>
+      <c r="D6">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B6,D$2)</f>
+        <v>4.529E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B6,E$2)</f>
+        <v>1527358636247</v>
+      </c>
+      <c r="F6" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B6,F$2)</f>
+        <v>4.5189999999999996E-3</v>
+      </c>
+      <c r="G6" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B6,G$2)</f>
+        <v>1527445036247</v>
+      </c>
+      <c r="H6" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B6,H$2)</f>
+        <v>-2133</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B6,I$2)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="J6" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B6,J$2)</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B7,C$2)</f>
+        <v>7.7615000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B7,D$2)</f>
+        <v>7.7644000000000005E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B7,E$2)</f>
+        <v>1527358636366</v>
+      </c>
+      <c r="F7" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B7,F$2)</f>
+        <v>7.7629500000000004E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B7,G$2)</f>
+        <v>1527445036366</v>
+      </c>
+      <c r="H7" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B7,H$2)</f>
+        <v>-2310</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B7,I$2)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B7,J$2)</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="3" t="str">
-        <f>RTD("rabbit",,"localhost","MODEL",$B3,F$8)</f>
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B8,C$2)</f>
+        <v>1.6133999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B8,D$2)</f>
+        <v>1.6163E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B8,E$2)</f>
+        <v>1527358636195</v>
+      </c>
+      <c r="F8" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B8,F$2)</f>
+        <v>1.61485E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B8,G$2)</f>
+        <v>1527445036195</v>
+      </c>
+      <c r="H8" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B8,H$2)</f>
+        <v>-2139</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B8,I$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="G9" s="6" t="str">
-        <f>RTD("rabbit",,"localhost","MODEL",$B3,G$8)</f>
+      <c r="J8" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$I$1,$B8,J$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="4">
-        <f>RTD("rabbit",,"localhost","MODEL",$B4,F$8)</f>
-        <v>603.76</v>
-      </c>
-      <c r="G10" s="6" t="str">
-        <f>RTD("rabbit",,"localhost","MODEL",$B4,G$8)</f>
-        <v>0001-01-01T00:00:00</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UnixDateime to excel datetime
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C318E4C6-6A90-4DBB-9A0B-209A142FD1F5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D58A7E-C098-4B85-AD0C-830F0A43C855}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Symbol</t>
   </si>
@@ -57,9 +57,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>ETHUSDT</t>
   </si>
   <si>
@@ -78,19 +75,22 @@
     <t>p</t>
   </si>
   <si>
-    <t>q</t>
-  </si>
-  <si>
     <t>BINANCE_AGGR_TRADE</t>
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,13 +192,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -206,7 +208,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,8 +233,8 @@
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCBTC</stp>
-        <stp>q</stp>
-        <tr r="J8" s="1"/>
+        <stp>p</stp>
+        <tr r="I8" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -240,17 +242,8 @@
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCBTC</stp>
-        <stp>p</stp>
-        <tr r="I8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>BINANCE_AGGR_TRADE</stp>
-        <stp>ETHBTC</stp>
-        <stp>q</stp>
-        <tr r="J7" s="1"/>
+        <stp>T</stp>
+        <tr r="J8" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -261,8 +254,35 @@
         <stp>p</stp>
         <tr r="I7" s="1"/>
       </tp>
-      <tp>
-        <v>118.01</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ETHBTC</stp>
+        <stp>T</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp>
+        <v>43247.735518773145</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>LTCUSDT</stp>
+        <stp>T</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+      <tp>
+        <v>43247.735524525466</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>BTCUSDT</stp>
+        <stp>T</stp>
+        <tr r="J3" s="1"/>
+      </tp>
+      <tp>
+        <v>117.01</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -271,16 +291,7 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>0.5</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>BINANCE_AGGR_TRADE</stp>
-        <stp>LTCUSDT</stp>
-        <stp>q</stp>
-        <tr r="J5" s="1"/>
-      </tp>
-      <tp>
-        <v>7310</v>
+        <v>7320</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -288,24 +299,6 @@
         <stp>p</stp>
         <tr r="I3" s="1"/>
       </tp>
-      <tp>
-        <v>5.5120000000000004E-3</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>BINANCE_AGGR_TRADE</stp>
-        <stp>BTCUSDT</stp>
-        <stp>q</stp>
-        <tr r="J3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>BINANCE_AGGR_TRADE</stp>
-        <stp>ZENBTC</stp>
-        <stp>q</stp>
-        <tr r="J6" s="1"/>
-      </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
         <stp/>
@@ -315,17 +308,26 @@
         <stp>p</stp>
         <tr r="I6" s="1"/>
       </tp>
-      <tp>
-        <v>7.0989999999999998E-2</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>ZENBTC</stp>
+        <stp>T</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+      <tp>
+        <v>43247.735583622685</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ETHUSDT</stp>
-        <stp>q</stp>
+        <stp>T</stp>
         <tr r="J4" s="1"/>
       </tp>
       <tp>
-        <v>567.70000000000005</v>
+        <v>564</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -334,7 +336,7 @@
         <tr r="I4" s="1"/>
       </tp>
       <tp>
-        <v>-2310</v>
+        <v>-2455</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -343,7 +345,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>7.7629500000000004E-2</v>
+        <v>7.7025499999999997E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -352,7 +354,7 @@
         <tr r="F7" s="1"/>
       </tp>
       <tp>
-        <v>1527445036366</v>
+        <v>43247.735589444441</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -361,7 +363,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp>
-        <v>-2139</v>
+        <v>-1837</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -370,7 +372,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>1.61485E-2</v>
+        <v>1.5986E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -379,7 +381,7 @@
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>1527445036195</v>
+        <v>43247.735582291665</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -388,7 +390,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>-2133</v>
+        <v>-2530</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -397,7 +399,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>4.5189999999999996E-3</v>
+        <v>4.4475000000000001E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -406,7 +408,7 @@
         <tr r="F6" s="1"/>
       </tp>
       <tp>
-        <v>1527445036247</v>
+        <v>43247.735590706019</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -415,16 +417,16 @@
         <tr r="G6" s="1"/>
       </tp>
       <tp>
-        <v>1527358636195</v>
+        <v>43247.735582291665</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>LTCBTC</stp>
-        <stp>O</stp>
+        <stp>C</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>1.6163E-2</v>
+        <v>1.5997000000000001E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -433,7 +435,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>1.6133999999999999E-2</v>
+        <v>1.5975E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -442,16 +444,16 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>1527358636366</v>
+        <v>43247.735589444441</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ETHBTC</stp>
-        <stp>O</stp>
+        <stp>C</stp>
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>7.7644000000000005E-2</v>
+        <v>7.7049999999999993E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -460,7 +462,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>7.7615000000000003E-2</v>
+        <v>7.7001E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -469,7 +471,7 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>7300.26</v>
+        <v>7315.04</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -478,7 +480,7 @@
         <tr r="C3" s="1"/>
       </tp>
       <tp>
-        <v>7311.66</v>
+        <v>7319.99</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -487,7 +489,7 @@
         <tr r="D3" s="1"/>
       </tp>
       <tp>
-        <v>118.19</v>
+        <v>117.01</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -496,7 +498,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>117.9</v>
+        <v>117</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -505,34 +507,34 @@
         <tr r="C5" s="1"/>
       </tp>
       <tp>
-        <v>1527358636327</v>
+        <v>43247.735590671298</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>BTCUSDT</stp>
+        <stp>C</stp>
+        <tr r="E3" s="1"/>
+      </tp>
+      <tp>
+        <v>43247.735576388892</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>LTCUSDT</stp>
-        <stp>O</stp>
+        <stp>C</stp>
         <tr r="E5" s="1"/>
       </tp>
       <tp>
-        <v>1527358636374</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>BINANCE</stp>
-        <stp>BTCUSDT</stp>
-        <stp>O</stp>
-        <tr r="E3" s="1"/>
-      </tp>
-      <tp>
-        <v>1527358636247</v>
+        <v>43247.735590706019</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ZENBTC</stp>
-        <stp>O</stp>
+        <stp>C</stp>
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>4.529E-3</v>
+        <v>4.4539999999999996E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -541,7 +543,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>4.509E-3</v>
+        <v>4.4409999999999996E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -550,7 +552,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>-2279</v>
+        <v>-2580</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -559,7 +561,7 @@
         <tr r="H4" s="1"/>
       </tp>
       <tp>
-        <v>567.40499999999997</v>
+        <v>564.125</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -568,7 +570,7 @@
         <tr r="F4" s="1"/>
       </tp>
       <tp>
-        <v>1527445036336</v>
+        <v>43247.735590925928</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -577,7 +579,7 @@
         <tr r="G4" s="1"/>
       </tp>
       <tp>
-        <v>567.73</v>
+        <v>564.25</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -586,7 +588,7 @@
         <tr r="D4" s="1"/>
       </tp>
       <tp>
-        <v>567.08000000000004</v>
+        <v>564</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -595,16 +597,16 @@
         <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>1527358636336</v>
+        <v>43247.735590925928</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
         <stp>ETHUSDT</stp>
-        <stp>O</stp>
+        <stp>C</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp>
-        <v>-2236</v>
+        <v>-2112</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -613,7 +615,7 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>-2317</v>
+        <v>-2558</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -622,7 +624,7 @@
         <tr r="H3" s="1"/>
       </tp>
       <tp>
-        <v>7305.96</v>
+        <v>7317.5150000000003</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -631,7 +633,7 @@
         <tr r="F3" s="1"/>
       </tp>
       <tp>
-        <v>118.045</v>
+        <v>117.005</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -640,7 +642,7 @@
         <tr r="F5" s="1"/>
       </tp>
       <tp>
-        <v>1527445036327</v>
+        <v>43247.735576388892</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -649,7 +651,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>1527445036374</v>
+        <v>43247.735590671298</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -673,7 +675,7 @@
     <tableColumn id="3" xr3:uid="{ECCD1A0A-D497-4C73-BD19-851157FDDFA6}" name="a">
       <calculatedColumnFormula>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{04F17769-55A0-4978-9AF0-73C1BFD079FB}" name="O" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{04F17769-55A0-4978-9AF0-73C1BFD079FB}" name="C" dataDxfId="0">
       <calculatedColumnFormula>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -981,16 +983,18 @@
   <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1002,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
@@ -1016,22 +1020,22 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -1043,35 +1047,35 @@
       </c>
       <c r="C3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>7300.26</v>
+        <v>7315.04</v>
       </c>
       <c r="D3">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>7311.66</v>
+        <v>7319.99</v>
       </c>
       <c r="E3" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
-        <v>1527358636374</v>
+        <v>43247.735590671298</v>
       </c>
       <c r="F3" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,F$2)</f>
-        <v>7305.96</v>
-      </c>
-      <c r="G3" s="3">
+        <v>7317.5150000000003</v>
+      </c>
+      <c r="G3" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,G$2)</f>
-        <v>1527445036374</v>
+        <v>43247.735590671298</v>
       </c>
       <c r="H3" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,H$2)</f>
-        <v>-2317</v>
+        <v>-2558</v>
       </c>
       <c r="I3" s="4">
         <f>RTD("rabbit",,"localhost",$I$1,$B3,I$2)</f>
-        <v>7310</v>
-      </c>
-      <c r="J3" s="4">
+        <v>7320</v>
+      </c>
+      <c r="J3" s="7">
         <f>RTD("rabbit",,"localhost",$I$1,$B3,J$2)</f>
-        <v>5.5120000000000004E-3</v>
+        <v>43247.735524525466</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
@@ -1079,185 +1083,185 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>567.08000000000004</v>
+        <v>564</v>
       </c>
       <c r="D4">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>567.73</v>
+        <v>564.25</v>
       </c>
       <c r="E4" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
-        <v>1527358636336</v>
+        <v>43247.735590925928</v>
       </c>
       <c r="F4" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,F$2)</f>
-        <v>567.40499999999997</v>
-      </c>
-      <c r="G4" s="3">
+        <v>564.125</v>
+      </c>
+      <c r="G4" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,G$2)</f>
-        <v>1527445036336</v>
+        <v>43247.735590925928</v>
       </c>
       <c r="H4" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,H$2)</f>
-        <v>-2279</v>
+        <v>-2580</v>
       </c>
       <c r="I4" s="4">
         <f>RTD("rabbit",,"localhost",$I$1,$B4,I$2)</f>
-        <v>567.70000000000005</v>
-      </c>
-      <c r="J4" s="4">
+        <v>564</v>
+      </c>
+      <c r="J4" s="7">
         <f>RTD("rabbit",,"localhost",$I$1,$B4,J$2)</f>
-        <v>7.0989999999999998E-2</v>
+        <v>43247.735583622685</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,C$2)</f>
-        <v>117.9</v>
+        <v>117</v>
       </c>
       <c r="D5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,D$2)</f>
-        <v>118.19</v>
+        <v>117.01</v>
       </c>
       <c r="E5" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,E$2)</f>
-        <v>1527358636327</v>
+        <v>43247.735576388892</v>
       </c>
       <c r="F5" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,F$2)</f>
-        <v>118.045</v>
-      </c>
-      <c r="G5" s="3">
+        <v>117.005</v>
+      </c>
+      <c r="G5" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,G$2)</f>
-        <v>1527445036327</v>
+        <v>43247.735576388892</v>
       </c>
       <c r="H5" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,H$2)</f>
-        <v>-2236</v>
+        <v>-2112</v>
       </c>
       <c r="I5" s="4">
         <f>RTD("rabbit",,"localhost",$I$1,$B5,I$2)</f>
-        <v>118.01</v>
-      </c>
-      <c r="J5" s="4">
+        <v>117.01</v>
+      </c>
+      <c r="J5" s="7">
         <f>RTD("rabbit",,"localhost",$I$1,$B5,J$2)</f>
-        <v>0.5</v>
+        <v>43247.735518773145</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,C$2)</f>
-        <v>4.509E-3</v>
+        <v>4.4409999999999996E-3</v>
       </c>
       <c r="D6">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,D$2)</f>
-        <v>4.529E-3</v>
+        <v>4.4539999999999996E-3</v>
       </c>
       <c r="E6" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,E$2)</f>
-        <v>1527358636247</v>
+        <v>43247.735590706019</v>
       </c>
       <c r="F6" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,F$2)</f>
-        <v>4.5189999999999996E-3</v>
-      </c>
-      <c r="G6" s="3">
+        <v>4.4475000000000001E-3</v>
+      </c>
+      <c r="G6" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,G$2)</f>
-        <v>1527445036247</v>
+        <v>43247.735590706019</v>
       </c>
       <c r="H6" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,H$2)</f>
-        <v>-2133</v>
+        <v>-2530</v>
       </c>
       <c r="I6" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B6,I$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J6" s="4" t="str">
+      <c r="J6" s="7" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B6,J$2)</f>
         <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,C$2)</f>
-        <v>7.7615000000000003E-2</v>
+        <v>7.7001E-2</v>
       </c>
       <c r="D7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,D$2)</f>
-        <v>7.7644000000000005E-2</v>
+        <v>7.7049999999999993E-2</v>
       </c>
       <c r="E7" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,E$2)</f>
-        <v>1527358636366</v>
+        <v>43247.735589444441</v>
       </c>
       <c r="F7" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,F$2)</f>
-        <v>7.7629500000000004E-2</v>
-      </c>
-      <c r="G7" s="3">
+        <v>7.7025499999999997E-2</v>
+      </c>
+      <c r="G7" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,G$2)</f>
-        <v>1527445036366</v>
+        <v>43247.735589444441</v>
       </c>
       <c r="H7" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,H$2)</f>
-        <v>-2310</v>
+        <v>-2455</v>
       </c>
       <c r="I7" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B7,I$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J7" s="4" t="str">
+      <c r="J7" s="7" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B7,J$2)</f>
         <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,C$2)</f>
-        <v>1.6133999999999999E-2</v>
+        <v>1.5975E-2</v>
       </c>
       <c r="D8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,D$2)</f>
-        <v>1.6163E-2</v>
+        <v>1.5997000000000001E-2</v>
       </c>
       <c r="E8" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,E$2)</f>
-        <v>1527358636195</v>
+        <v>43247.735582291665</v>
       </c>
       <c r="F8" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,F$2)</f>
-        <v>1.61485E-2</v>
-      </c>
-      <c r="G8" s="3">
+        <v>1.5986E-2</v>
+      </c>
+      <c r="G8" s="6">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,G$2)</f>
-        <v>1527445036195</v>
+        <v>43247.735582291665</v>
       </c>
       <c r="H8" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,H$2)</f>
-        <v>-2139</v>
+        <v>-1837</v>
       </c>
       <c r="I8" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B8,I$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J8" s="4" t="str">
+      <c r="J8" s="7" t="str">
         <f>RTD("rabbit",,"localhost",$I$1,$B8,J$2)</f>
         <v>&lt;?&gt;</v>
       </c>

</xml_diff>

<commit_message>
Add CLOCK and LAST_RTD
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D58A7E-C098-4B85-AD0C-830F0A43C855}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA19C3AD-1D3D-4982-823B-E2C23B30C7B3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="CLOCK">Sheet1!$I$1</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Symbol</t>
   </si>
@@ -54,9 +58,6 @@
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>ETHUSDT</t>
   </si>
   <si>
@@ -82,14 +83,20 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>BNBUSDT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="mm:ss.000"/>
+    <numFmt numFmtId="166" formatCode="s.000"/>
+    <numFmt numFmtId="167" formatCode="h:mm:ss.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -192,15 +199,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -208,7 +220,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -227,6 +239,18 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="rabbit">
+      <tp>
+        <v>43249.921993599535</v>
+        <stp/>
+        <stp>LAST_RTD</stp>
+        <tr r="H1" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.922391666667</v>
+        <stp/>
+        <stp>CLOCK</stp>
+        <tr r="I1" s="1"/>
+      </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
         <stp/>
@@ -234,7 +258,7 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCBTC</stp>
         <stp>p</stp>
-        <tr r="I8" s="1"/>
+        <tr r="K8" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -243,7 +267,7 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCBTC</stp>
         <stp>T</stp>
-        <tr r="J8" s="1"/>
+        <tr r="L8" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -252,7 +276,7 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ETHBTC</stp>
         <stp>p</stp>
-        <tr r="I7" s="1"/>
+        <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -261,43 +285,61 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ETHBTC</stp>
         <stp>T</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-      <tp>
-        <v>43247.735518773145</v>
+        <tr r="L7" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921999189814</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCUSDT</stp>
         <stp>T</stp>
-        <tr r="J5" s="1"/>
-      </tp>
-      <tp>
-        <v>43247.735524525466</v>
+        <tr r="L5" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921997407408</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>BTCUSDT</stp>
         <stp>T</stp>
-        <tr r="J3" s="1"/>
-      </tp>
-      <tp>
-        <v>117.01</v>
+        <tr r="L3" s="1"/>
+      </tp>
+      <tp>
+        <v>121.47</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>LTCUSDT</stp>
         <stp>p</stp>
-        <tr r="I5" s="1"/>
-      </tp>
-      <tp>
-        <v>7320</v>
+        <tr r="K5" s="1"/>
+      </tp>
+      <tp>
+        <v>7528</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>BTCUSDT</stp>
         <stp>p</stp>
-        <tr r="I3" s="1"/>
+        <tr r="K3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>BNBUSDT</stp>
+        <stp>T</stp>
+        <tr r="L9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE_AGGR_TRADE</stp>
+        <stp>BNBUSDT</stp>
+        <stp>p</stp>
+        <tr r="K9" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -306,7 +348,7 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ZENBTC</stp>
         <stp>p</stp>
-        <tr r="I6" s="1"/>
+        <tr r="K6" s="1"/>
       </tp>
       <tp t="s">
         <v>&lt;?&gt;</v>
@@ -315,37 +357,28 @@
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ZENBTC</stp>
         <stp>T</stp>
-        <tr r="J6" s="1"/>
-      </tp>
-      <tp>
-        <v>43247.735583622685</v>
+        <tr r="L6" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921958564817</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ETHUSDT</stp>
         <stp>T</stp>
-        <tr r="J4" s="1"/>
-      </tp>
-      <tp>
-        <v>564</v>
+        <tr r="L4" s="1"/>
+      </tp>
+      <tp>
+        <v>581.34</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
         <stp>ETHUSDT</stp>
         <stp>p</stp>
-        <tr r="I4" s="1"/>
-      </tp>
-      <tp>
-        <v>-2455</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>ETHBTC</stp>
-        <stp>t</stp>
-        <tr r="H7" s="1"/>
-      </tp>
-      <tp>
-        <v>7.7025499999999997E-2</v>
+        <tr r="K4" s="1"/>
+      </tp>
+      <tp>
+        <v>7.7218999999999996E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -354,25 +387,25 @@
         <tr r="F7" s="1"/>
       </tp>
       <tp>
-        <v>43247.735589444441</v>
+        <v>43249.921900787034</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>T</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921904606483</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>ETHBTC</stp>
         <stp>C</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-      <tp>
-        <v>-1837</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>LTCBTC</stp>
-        <stp>t</stp>
-        <tr r="H8" s="1"/>
-      </tp>
-      <tp>
-        <v>1.5986E-2</v>
+        <tr r="H7" s="1"/>
+      </tp>
+      <tp>
+        <v>1.6138E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -381,25 +414,25 @@
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>43247.735582291665</v>
+        <v>43249.921888935183</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>T</stp>
+        <tr r="G8" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921887187498</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>LTCBTC</stp>
         <stp>C</stp>
-        <tr r="G8" s="1"/>
-      </tp>
-      <tp>
-        <v>-2530</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>ZENBTC</stp>
-        <stp>t</stp>
-        <tr r="H6" s="1"/>
-      </tp>
-      <tp>
-        <v>4.4475000000000001E-3</v>
+        <tr r="H8" s="1"/>
+      </tp>
+      <tp>
+        <v>4.1460000000000004E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -408,16 +441,25 @@
         <tr r="F6" s="1"/>
       </tp>
       <tp>
-        <v>43247.735590706019</v>
+        <v>43249.921901377318</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>T</stp>
+        <tr r="G6" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921900162037</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>ZENBTC</stp>
         <stp>C</stp>
-        <tr r="G6" s="1"/>
-      </tp>
-      <tp>
-        <v>43247.735582291665</v>
+        <tr r="H6" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921970763891</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -426,7 +468,7 @@
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>1.5997000000000001E-2</v>
+        <v>1.6140000000000002E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -435,7 +477,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>1.5975E-2</v>
+        <v>1.6136000000000001E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -444,7 +486,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43247.735589444441</v>
+        <v>43249.921997523146</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -453,7 +495,7 @@
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>7.7049999999999993E-2</v>
+        <v>7.7248999999999998E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -462,7 +504,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>7.7001E-2</v>
+        <v>7.7188000000000007E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -471,7 +513,34 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>7315.04</v>
+        <v>12.712</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>BNBUSDT</stp>
+        <stp>b</stp>
+        <tr r="C9" s="1"/>
+      </tp>
+      <tp>
+        <v>12.729900000000001</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>BNBUSDT</stp>
+        <stp>a</stp>
+        <tr r="D9" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.92199091435</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>BINANCE</stp>
+        <stp>BNBUSDT</stp>
+        <stp>C</stp>
+        <tr r="E9" s="1"/>
+      </tp>
+      <tp>
+        <v>7523.6</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -480,7 +549,7 @@
         <tr r="C3" s="1"/>
       </tp>
       <tp>
-        <v>7319.99</v>
+        <v>7528</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -489,7 +558,7 @@
         <tr r="D3" s="1"/>
       </tp>
       <tp>
-        <v>117.01</v>
+        <v>121.47</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -498,7 +567,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>117</v>
+        <v>121.29</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -507,7 +576,7 @@
         <tr r="C5" s="1"/>
       </tp>
       <tp>
-        <v>43247.735590671298</v>
+        <v>43249.921997407408</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -516,7 +585,7 @@
         <tr r="E3" s="1"/>
       </tp>
       <tp>
-        <v>43247.735576388892</v>
+        <v>43249.921992384261</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -525,7 +594,7 @@
         <tr r="E5" s="1"/>
       </tp>
       <tp>
-        <v>43247.735590706019</v>
+        <v>43249.921987037036</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -534,7 +603,7 @@
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>4.4539999999999996E-3</v>
+        <v>4.1549999999999998E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -543,7 +612,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>4.4409999999999996E-3</v>
+        <v>4.1359999999999999E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -552,16 +621,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>-2580</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>ETHUSDT</stp>
-        <stp>t</stp>
-        <tr r="H4" s="1"/>
-      </tp>
-      <tp>
-        <v>564.125</v>
+        <v>581.55499999999995</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -570,16 +630,25 @@
         <tr r="F4" s="1"/>
       </tp>
       <tp>
-        <v>43247.735590925928</v>
+        <v>43249.921900810186</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>ETHUSDT</stp>
+        <stp>T</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921905138886</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>ETHUSDT</stp>
         <stp>C</stp>
-        <tr r="G4" s="1"/>
-      </tp>
-      <tp>
-        <v>564.25</v>
+        <tr r="H4" s="1"/>
+      </tp>
+      <tp>
+        <v>581.77</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -588,7 +657,7 @@
         <tr r="D4" s="1"/>
       </tp>
       <tp>
-        <v>564</v>
+        <v>581.34</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -597,7 +666,7 @@
         <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>43247.735590925928</v>
+        <v>43249.921990138886</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -606,25 +675,7 @@
         <tr r="E4" s="1"/>
       </tp>
       <tp>
-        <v>-2112</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>LTCUSDT</stp>
-        <stp>t</stp>
-        <tr r="H5" s="1"/>
-      </tp>
-      <tp>
-        <v>-2558</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>MODEL</stp>
-        <stp>BTCUSDT</stp>
-        <stp>t</stp>
-        <tr r="H3" s="1"/>
-      </tp>
-      <tp>
-        <v>7317.5150000000003</v>
+        <v>7525.2650000000003</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -633,7 +684,7 @@
         <tr r="F3" s="1"/>
       </tp>
       <tp>
-        <v>117.005</v>
+        <v>121.38</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -642,22 +693,67 @@
         <tr r="F5" s="1"/>
       </tp>
       <tp>
-        <v>43247.735576388892</v>
+        <v>43249.921901111113</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>T</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921900810186</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BTCUSDT</stp>
+        <stp>T</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921901145834</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>LTCUSDT</stp>
         <stp>C</stp>
-        <tr r="G5" s="1"/>
-      </tp>
-      <tp>
-        <v>43247.735590671298</v>
+        <tr r="H5" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921903125003</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>BTCUSDT</stp>
         <stp>C</stp>
-        <tr r="G3" s="1"/>
+        <tr r="H3" s="1"/>
+      </tp>
+      <tp>
+        <v>12.72085</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BNBUSDT</stp>
+        <stp>m</stp>
+        <tr r="F9" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.921889131947</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BNBUSDT</stp>
+        <stp>T</stp>
+        <tr r="G9" s="1"/>
+      </tp>
+      <tp>
+        <v>43249.92188681713</v>
+        <stp/>
+        <stp>localhost</stp>
+        <stp>MODEL</stp>
+        <stp>BNBUSDT</stp>
+        <stp>C</stp>
+        <tr r="H9" s="1"/>
       </tp>
     </main>
   </volType>
@@ -665,8 +761,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:E8" totalsRowShown="0">
-  <autoFilter ref="B2:E8" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C0D435-FF19-4363-81EE-23749C726FA3}" name="Table1" displayName="Table1" ref="B2:E9" totalsRowShown="0">
+  <autoFilter ref="B2:E9" xr:uid="{F5CE4B6E-5208-48A0-8103-68B82B26FD82}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4684B3D0-E19D-45C0-AF8D-58548797FDAF}" name="Symbol"/>
     <tableColumn id="2" xr3:uid="{025AE9D2-02E3-4A4E-9988-5BB682835FAE}" name="b">
@@ -980,36 +1076,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35C332D-6131-427D-B374-A8266C368C7A}">
-  <dimension ref="B1:L8"/>
+  <dimension ref="B1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
+      <c r="H1" s="10">
+        <f>RTD("rabbit",,"LAST_RTD")</f>
+        <v>43249.921993599535</v>
+      </c>
+      <c r="I1" s="10">
+        <f>RTD("rabbit",,"CLOCK")</f>
+        <v>43249.922391666667</v>
+      </c>
+      <c r="J1" s="8">
+        <f>CLOCK-H1</f>
+        <v>3.9806713175494224E-4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -1029,241 +1141,346 @@
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
       </c>
       <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>7315.04</v>
-      </c>
-      <c r="D3">
+        <v>7523.6</v>
+      </c>
+      <c r="D3" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>7319.99</v>
+        <v>7528</v>
       </c>
       <c r="E3" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
-        <v>43247.735590671298</v>
+        <v>43249.921997407408</v>
       </c>
       <c r="F3" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,F$2)</f>
-        <v>7317.5150000000003</v>
-      </c>
-      <c r="G3" s="6">
+        <v>7525.2650000000003</v>
+      </c>
+      <c r="G3" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,G$2)</f>
-        <v>43247.735590671298</v>
-      </c>
-      <c r="H3" s="3">
+        <v>43249.921900810186</v>
+      </c>
+      <c r="H3" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,H$2)</f>
-        <v>-2558</v>
-      </c>
-      <c r="I3" s="4">
-        <f>RTD("rabbit",,"localhost",$I$1,$B3,I$2)</f>
-        <v>7320</v>
-      </c>
-      <c r="J3" s="7">
-        <f>RTD("rabbit",,"localhost",$I$1,$B3,J$2)</f>
-        <v>43247.735524525466</v>
-      </c>
-      <c r="L3" t="s">
+        <v>43249.921903125003</v>
+      </c>
+      <c r="I3" s="7">
+        <f>(H3-G3)*86400000</f>
+        <v>200.00017248094082</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" ref="J3:J8" si="0">(CLOCK-G3)</f>
+        <v>4.9085648061009124E-4</v>
+      </c>
+      <c r="K3" s="4">
+        <f>RTD("rabbit",,"localhost",$K$1,$B3,K$2)</f>
+        <v>7528</v>
+      </c>
+      <c r="L3" s="6">
+        <f>RTD("rabbit",,"localhost",$K$1,$B3,L$2)</f>
+        <v>43249.921997407408</v>
+      </c>
+      <c r="N3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>564</v>
-      </c>
-      <c r="D4">
+        <v>581.34</v>
+      </c>
+      <c r="D4" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>564.25</v>
+        <v>581.77</v>
       </c>
       <c r="E4" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
-        <v>43247.735590925928</v>
+        <v>43249.921990138886</v>
       </c>
       <c r="F4" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,F$2)</f>
-        <v>564.125</v>
-      </c>
-      <c r="G4" s="6">
+        <v>581.55499999999995</v>
+      </c>
+      <c r="G4" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,G$2)</f>
-        <v>43247.735590925928</v>
-      </c>
-      <c r="H4" s="3">
+        <v>43249.921900810186</v>
+      </c>
+      <c r="H4" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,H$2)</f>
-        <v>-2580</v>
-      </c>
-      <c r="I4" s="4">
-        <f>RTD("rabbit",,"localhost",$I$1,$B4,I$2)</f>
-        <v>564</v>
-      </c>
-      <c r="J4" s="7">
-        <f>RTD("rabbit",,"localhost",$I$1,$B4,J$2)</f>
-        <v>43247.735583622685</v>
+        <v>43249.921905138886</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" ref="I4:I8" si="1">(H4-G4)*86400000</f>
+        <v>373.99968132376671</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="0"/>
+        <v>4.9085648061009124E-4</v>
+      </c>
+      <c r="K4" s="4">
+        <f>RTD("rabbit",,"localhost",$K$1,$B4,K$2)</f>
+        <v>581.34</v>
+      </c>
+      <c r="L4" s="6">
+        <f>RTD("rabbit",,"localhost",$K$1,$B4,L$2)</f>
+        <v>43249.921958564817</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,C$2)</f>
-        <v>117</v>
-      </c>
-      <c r="D5">
+        <v>121.29</v>
+      </c>
+      <c r="D5" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,D$2)</f>
-        <v>117.01</v>
+        <v>121.47</v>
       </c>
       <c r="E5" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,E$2)</f>
-        <v>43247.735576388892</v>
+        <v>43249.921992384261</v>
       </c>
       <c r="F5" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,F$2)</f>
-        <v>117.005</v>
-      </c>
-      <c r="G5" s="6">
+        <v>121.38</v>
+      </c>
+      <c r="G5" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,G$2)</f>
-        <v>43247.735576388892</v>
-      </c>
-      <c r="H5" s="3">
+        <v>43249.921901111113</v>
+      </c>
+      <c r="H5" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,H$2)</f>
-        <v>-2112</v>
-      </c>
-      <c r="I5" s="4">
-        <f>RTD("rabbit",,"localhost",$I$1,$B5,I$2)</f>
-        <v>117.01</v>
-      </c>
-      <c r="J5" s="7">
-        <f>RTD("rabbit",,"localhost",$I$1,$B5,J$2)</f>
-        <v>43247.735518773145</v>
+        <v>43249.921901145834</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="1"/>
+        <v>2.9998831450939178</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="0"/>
+        <v>4.9055555427912623E-4</v>
+      </c>
+      <c r="K5" s="4">
+        <f>RTD("rabbit",,"localhost",$K$1,$B5,K$2)</f>
+        <v>121.47</v>
+      </c>
+      <c r="L5" s="6">
+        <f>RTD("rabbit",,"localhost",$K$1,$B5,L$2)</f>
+        <v>43249.921999189814</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,C$2)</f>
-        <v>4.4409999999999996E-3</v>
-      </c>
-      <c r="D6">
+        <v>4.1359999999999999E-3</v>
+      </c>
+      <c r="D6" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,D$2)</f>
-        <v>4.4539999999999996E-3</v>
+        <v>4.1549999999999998E-3</v>
       </c>
       <c r="E6" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,E$2)</f>
-        <v>43247.735590706019</v>
+        <v>43249.921987037036</v>
       </c>
       <c r="F6" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,F$2)</f>
-        <v>4.4475000000000001E-3</v>
-      </c>
-      <c r="G6" s="6">
+        <v>4.1460000000000004E-3</v>
+      </c>
+      <c r="G6" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,G$2)</f>
-        <v>43247.735590706019</v>
-      </c>
-      <c r="H6" s="3">
+        <v>43249.921901377318</v>
+      </c>
+      <c r="H6" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,H$2)</f>
-        <v>-2530</v>
-      </c>
-      <c r="I6" s="4" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B6,I$2)</f>
+        <v>43249.921900162037</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="1"/>
+        <v>-105.00031057745218</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="0"/>
+        <v>4.902893488178961E-4</v>
+      </c>
+      <c r="K6" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B6,K$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J6" s="7" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B6,J$2)</f>
+      <c r="L6" s="6" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B6,L$2)</f>
         <v>&lt;?&gt;</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,C$2)</f>
-        <v>7.7001E-2</v>
+        <v>7.7188000000000007E-2</v>
       </c>
       <c r="D7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,D$2)</f>
-        <v>7.7049999999999993E-2</v>
+        <v>7.7248999999999998E-2</v>
       </c>
       <c r="E7" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,E$2)</f>
-        <v>43247.735589444441</v>
+        <v>43249.921997523146</v>
       </c>
       <c r="F7" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,F$2)</f>
-        <v>7.7025499999999997E-2</v>
-      </c>
-      <c r="G7" s="6">
+        <v>7.7218999999999996E-2</v>
+      </c>
+      <c r="G7" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,G$2)</f>
-        <v>43247.735589444441</v>
-      </c>
-      <c r="H7" s="3">
+        <v>43249.921900787034</v>
+      </c>
+      <c r="H7" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,H$2)</f>
-        <v>-2455</v>
-      </c>
-      <c r="I7" s="4" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B7,I$2)</f>
+        <v>43249.921904606483</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>330.00034745782614</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="0"/>
+        <v>4.9087963270721957E-4</v>
+      </c>
+      <c r="K7" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B7,K$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J7" s="7" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B7,J$2)</f>
+      <c r="L7" s="6" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B7,L$2)</f>
         <v>&lt;?&gt;</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,C$2)</f>
-        <v>1.5975E-2</v>
+        <v>1.6136000000000001E-2</v>
       </c>
       <c r="D8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,D$2)</f>
-        <v>1.5997000000000001E-2</v>
+        <v>1.6140000000000002E-2</v>
       </c>
       <c r="E8" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,E$2)</f>
-        <v>43247.735582291665</v>
+        <v>43249.921970763891</v>
       </c>
       <c r="F8" s="3">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,F$2)</f>
-        <v>1.5986E-2</v>
-      </c>
-      <c r="G8" s="6">
+        <v>1.6138E-2</v>
+      </c>
+      <c r="G8" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,G$2)</f>
-        <v>43247.735582291665</v>
-      </c>
-      <c r="H8" s="3">
+        <v>43249.921888935183</v>
+      </c>
+      <c r="H8" s="11">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,H$2)</f>
-        <v>-1837</v>
-      </c>
-      <c r="I8" s="4" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B8,I$2)</f>
+        <v>43249.921887187498</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>-150.99998563528061</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="0"/>
+        <v>5.0273148372070864E-4</v>
+      </c>
+      <c r="K8" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B8,K$2)</f>
         <v>&lt;?&gt;</v>
       </c>
-      <c r="J8" s="7" t="str">
-        <f>RTD("rabbit",,"localhost",$I$1,$B8,J$2)</f>
+      <c r="L8" s="6" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B8,L$2)</f>
         <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B9,C$2)</f>
+        <v>12.712</v>
+      </c>
+      <c r="D9">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B9,D$2)</f>
+        <v>12.729900000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <f>RTD("rabbit",,"localhost","BINANCE",$B9,E$2)</f>
+        <v>43249.92199091435</v>
+      </c>
+      <c r="F9" s="3">
+        <f>RTD("rabbit",,"localhost","MODEL",$B9,F$2)</f>
+        <v>12.72085</v>
+      </c>
+      <c r="G9" s="11">
+        <f>RTD("rabbit",,"localhost","MODEL",$B9,G$2)</f>
+        <v>43249.921889131947</v>
+      </c>
+      <c r="H9" s="11">
+        <f>RTD("rabbit",,"localhost","MODEL",$B9,H$2)</f>
+        <v>43249.92188681713</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" ref="I9" si="2">(H9-G9)*86400000</f>
+        <v>-200.00017248094082</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" ref="J9" si="3">(CLOCK-G9)</f>
+        <v>5.0253471999894828E-4</v>
+      </c>
+      <c r="K9" s="4" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B9,K$2)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="L9" s="6" t="str">
+        <f>RTD("rabbit",,"localhost",$K$1,$B9,L$2)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="10">
+        <f>MIN(J3:J8)</f>
+        <v>4.902893488178961E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>C3*0.001</f>
+        <v>7.523600000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1273,4 +1490,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11374B4B-BAF3-4DE9-8F2E-E0D2F1C20227}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implement _dirtyMap, more effecient
</commit_message>
<xml_diff>
--- a/doc/Test.xlsx
+++ b/doc/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Crypto-XLS\rabbit-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA19C3AD-1D3D-4982-823B-E2C23B30C7B3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA71CC2C-D6BC-454F-AA66-45E287CFFF33}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{E8EE775B-36F4-45BC-A6D4-0C0867A090A7}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Symbol</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>BNBUSDT</t>
+  </si>
+  <si>
+    <t>rabbit</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -194,12 +203,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -213,6 +235,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -240,13 +264,13 @@
   <volType type="realTimeData">
     <main first="rabbit">
       <tp>
-        <v>43249.921993599535</v>
+        <v>43250.778604976855</v>
         <stp/>
         <stp>LAST_RTD</stp>
         <tr r="H1" s="1"/>
       </tp>
       <tp>
-        <v>43249.922391666667</v>
+        <v>43250.778606250002</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="I1" s="1"/>
@@ -288,7 +312,7 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>43249.921999189814</v>
+        <v>43250.778610671296</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -297,7 +321,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>43249.921997407408</v>
+        <v>43250.77859480324</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -306,7 +330,7 @@
         <tr r="L3" s="1"/>
       </tp>
       <tp>
-        <v>121.47</v>
+        <v>116.76</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -315,7 +339,7 @@
         <tr r="K5" s="1"/>
       </tp>
       <tp>
-        <v>7528</v>
+        <v>7345.6</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -360,7 +384,7 @@
         <tr r="L6" s="1"/>
       </tp>
       <tp>
-        <v>43249.921958564817</v>
+        <v>43250.778517500003</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -369,7 +393,7 @@
         <tr r="L4" s="1"/>
       </tp>
       <tp>
-        <v>581.34</v>
+        <v>551</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE_AGGR_TRADE</stp>
@@ -377,8 +401,32 @@
         <stp>p</stp>
         <tr r="K4" s="1"/>
       </tp>
-      <tp>
-        <v>7.7218999999999996E-2</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>BTCUSDT</stp>
+        <stp>CLOSE</stp>
+        <tr r="D14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>CLOSE</stp>
+        <tr r="D16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>BNBUSDT</stp>
+        <stp>CLOSE</stp>
+        <tr r="D20" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -386,8 +434,8 @@
         <stp>m</stp>
         <tr r="F7" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921900787034</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -395,8 +443,8 @@
         <stp>T</stp>
         <tr r="G7" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921904606483</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -404,8 +452,8 @@
         <stp>C</stp>
         <tr r="H7" s="1"/>
       </tp>
-      <tp>
-        <v>1.6138E-2</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -413,8 +461,8 @@
         <stp>m</stp>
         <tr r="F8" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921888935183</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -422,8 +470,8 @@
         <stp>T</stp>
         <tr r="G8" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921887187498</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -431,8 +479,16 @@
         <stp>C</stp>
         <tr r="H8" s="1"/>
       </tp>
-      <tp>
-        <v>4.1460000000000004E-3</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ETHUSDT</stp>
+        <stp>CLOSE</stp>
+        <tr r="D15" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -440,8 +496,8 @@
         <stp>m</stp>
         <tr r="F6" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921901377318</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -449,8 +505,8 @@
         <stp>T</stp>
         <tr r="G6" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921900162037</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -459,7 +515,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>43249.921970763891</v>
+        <v>43250.778599166668</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -468,7 +524,7 @@
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>1.6140000000000002E-2</v>
+        <v>1.5890999999999999E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -477,7 +533,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>1.6136000000000001E-2</v>
+        <v>1.5890000000000001E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -486,7 +542,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43249.921997523146</v>
+        <v>43250.778605717591</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -495,7 +551,7 @@
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>7.7248999999999998E-2</v>
+        <v>7.5059000000000001E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -504,7 +560,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>7.7188000000000007E-2</v>
+        <v>7.5005000000000002E-2</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -512,8 +568,56 @@
         <stp>b</stp>
         <tr r="C7" s="1"/>
       </tp>
-      <tp>
-        <v>12.712</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ETHUSDT</stp>
+        <stp>OPEN</stp>
+        <tr r="C15" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>LTCUSDT</stp>
+        <stp>OPEN</stp>
+        <tr r="C16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>BTCUSDT</stp>
+        <stp>OPEN</stp>
+        <tr r="C14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>OPEN</stp>
+        <tr r="C18" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>CLOSE</stp>
+        <tr r="D17" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>OPEN</stp>
+        <tr r="C19" s="1"/>
+      </tp>
+      <tp>
+        <v>12.371600000000001</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -522,7 +626,7 @@
         <tr r="C9" s="1"/>
       </tp>
       <tp>
-        <v>12.729900000000001</v>
+        <v>12.39</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -531,7 +635,7 @@
         <tr r="D9" s="1"/>
       </tp>
       <tp>
-        <v>43249.92199091435</v>
+        <v>43250.778593726849</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -540,7 +644,7 @@
         <tr r="E9" s="1"/>
       </tp>
       <tp>
-        <v>7523.6</v>
+        <v>7340.12</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -549,7 +653,7 @@
         <tr r="C3" s="1"/>
       </tp>
       <tp>
-        <v>7528</v>
+        <v>7345.6</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -558,7 +662,7 @@
         <tr r="D3" s="1"/>
       </tp>
       <tp>
-        <v>121.47</v>
+        <v>116.76</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -567,7 +671,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>121.29</v>
+        <v>116.68</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -576,7 +680,7 @@
         <tr r="C5" s="1"/>
       </tp>
       <tp>
-        <v>43249.921997407408</v>
+        <v>43250.778601840277</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -585,7 +689,7 @@
         <tr r="E3" s="1"/>
       </tp>
       <tp>
-        <v>43249.921992384261</v>
+        <v>43250.778600613427</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -594,7 +698,7 @@
         <tr r="E5" s="1"/>
       </tp>
       <tp>
-        <v>43249.921987037036</v>
+        <v>43250.778602685183</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -603,7 +707,7 @@
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>4.1549999999999998E-3</v>
+        <v>4.1000000000000003E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -612,7 +716,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>4.1359999999999999E-3</v>
+        <v>4.0800000000000003E-3</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -620,8 +724,8 @@
         <stp>b</stp>
         <tr r="C6" s="1"/>
       </tp>
-      <tp>
-        <v>581.55499999999995</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -629,8 +733,8 @@
         <stp>m</stp>
         <tr r="F4" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921900810186</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -638,8 +742,8 @@
         <stp>T</stp>
         <tr r="G4" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921905138886</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -648,7 +752,7 @@
         <tr r="H4" s="1"/>
       </tp>
       <tp>
-        <v>581.77</v>
+        <v>551</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -657,7 +761,7 @@
         <tr r="D4" s="1"/>
       </tp>
       <tp>
-        <v>581.34</v>
+        <v>550.61</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -666,7 +770,7 @@
         <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>43249.921990138886</v>
+        <v>43250.778597569442</v>
         <stp/>
         <stp>localhost</stp>
         <stp>BINANCE</stp>
@@ -674,8 +778,8 @@
         <stp>C</stp>
         <tr r="E4" s="1"/>
       </tp>
-      <tp>
-        <v>7525.2650000000003</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -683,8 +787,8 @@
         <stp>m</stp>
         <tr r="F3" s="1"/>
       </tp>
-      <tp>
-        <v>121.38</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -692,8 +796,8 @@
         <stp>m</stp>
         <tr r="F5" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921901111113</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -701,8 +805,8 @@
         <stp>T</stp>
         <tr r="G5" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921900810186</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -710,8 +814,8 @@
         <stp>T</stp>
         <tr r="G3" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921901145834</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -719,8 +823,8 @@
         <stp>C</stp>
         <tr r="H5" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921903125003</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -728,8 +832,16 @@
         <stp>C</stp>
         <tr r="H3" s="1"/>
       </tp>
-      <tp>
-        <v>12.72085</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ZENBTC</stp>
+        <stp>OPEN</stp>
+        <tr r="C17" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -737,8 +849,8 @@
         <stp>m</stp>
         <tr r="F9" s="1"/>
       </tp>
-      <tp>
-        <v>43249.921889131947</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
@@ -746,14 +858,38 @@
         <stp>T</stp>
         <tr r="G9" s="1"/>
       </tp>
-      <tp>
-        <v>43249.92188681713</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>MODEL</stp>
         <stp>BNBUSDT</stp>
         <stp>C</stp>
         <tr r="H9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>ETHBTC</stp>
+        <stp>CLOSE</stp>
+        <tr r="D18" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>LTCBTC</stp>
+        <stp>CLOSE</stp>
+        <tr r="D19" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>MODEL</stp>
+        <stp>BNBUSDT</stp>
+        <stp>OPEN</stp>
+        <tr r="C20" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1076,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35C332D-6131-427D-B374-A8266C368C7A}">
-  <dimension ref="B1:N15"/>
+  <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,15 +1243,15 @@
       </c>
       <c r="H1" s="10">
         <f>RTD("rabbit",,"LAST_RTD")</f>
-        <v>43249.921993599535</v>
+        <v>43250.778604976855</v>
       </c>
       <c r="I1" s="10">
         <f>RTD("rabbit",,"CLOCK")</f>
-        <v>43249.922391666667</v>
+        <v>43250.778606250002</v>
       </c>
       <c r="J1" s="8">
         <f>CLOCK-H1</f>
-        <v>3.9806713175494224E-4</v>
+        <v>1.2731470633298159E-6</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
@@ -1159,43 +1295,43 @@
       </c>
       <c r="C3" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,C$2)</f>
-        <v>7523.6</v>
+        <v>7340.12</v>
       </c>
       <c r="D3" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,D$2)</f>
-        <v>7528</v>
+        <v>7345.6</v>
       </c>
       <c r="E3" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B3,E$2)</f>
-        <v>43249.921997407408</v>
-      </c>
-      <c r="F3" s="3">
+        <v>43250.778601840277</v>
+      </c>
+      <c r="F3" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,F$2)</f>
-        <v>7525.2650000000003</v>
-      </c>
-      <c r="G3" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G3" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,G$2)</f>
-        <v>43249.921900810186</v>
-      </c>
-      <c r="H3" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H3" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B3,H$2)</f>
-        <v>43249.921903125003</v>
-      </c>
-      <c r="I3" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I3" s="7" t="e">
         <f>(H3-G3)*86400000</f>
-        <v>200.00017248094082</v>
-      </c>
-      <c r="J3" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="9" t="e">
         <f t="shared" ref="J3:J8" si="0">(CLOCK-G3)</f>
-        <v>4.9085648061009124E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K3" s="4">
         <f>RTD("rabbit",,"localhost",$K$1,$B3,K$2)</f>
-        <v>7528</v>
+        <v>7345.6</v>
       </c>
       <c r="L3" s="6">
         <f>RTD("rabbit",,"localhost",$K$1,$B3,L$2)</f>
-        <v>43249.921997407408</v>
+        <v>43250.77859480324</v>
       </c>
       <c r="N3" t="s">
         <v>7</v>
@@ -1207,43 +1343,43 @@
       </c>
       <c r="C4" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,C$2)</f>
-        <v>581.34</v>
+        <v>550.61</v>
       </c>
       <c r="D4" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,D$2)</f>
-        <v>581.77</v>
+        <v>551</v>
       </c>
       <c r="E4" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B4,E$2)</f>
-        <v>43249.921990138886</v>
-      </c>
-      <c r="F4" s="3">
+        <v>43250.778597569442</v>
+      </c>
+      <c r="F4" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,F$2)</f>
-        <v>581.55499999999995</v>
-      </c>
-      <c r="G4" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G4" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,G$2)</f>
-        <v>43249.921900810186</v>
-      </c>
-      <c r="H4" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H4" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B4,H$2)</f>
-        <v>43249.921905138886</v>
-      </c>
-      <c r="I4" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I4" s="7" t="e">
         <f t="shared" ref="I4:I8" si="1">(H4-G4)*86400000</f>
-        <v>373.99968132376671</v>
-      </c>
-      <c r="J4" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4" s="9" t="e">
         <f t="shared" si="0"/>
-        <v>4.9085648061009124E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K4" s="4">
         <f>RTD("rabbit",,"localhost",$K$1,$B4,K$2)</f>
-        <v>581.34</v>
+        <v>551</v>
       </c>
       <c r="L4" s="6">
         <f>RTD("rabbit",,"localhost",$K$1,$B4,L$2)</f>
-        <v>43249.921958564817</v>
+        <v>43250.778517500003</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -1252,43 +1388,43 @@
       </c>
       <c r="C5" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,C$2)</f>
-        <v>121.29</v>
+        <v>116.68</v>
       </c>
       <c r="D5" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,D$2)</f>
-        <v>121.47</v>
+        <v>116.76</v>
       </c>
       <c r="E5" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B5,E$2)</f>
-        <v>43249.921992384261</v>
-      </c>
-      <c r="F5" s="3">
+        <v>43250.778600613427</v>
+      </c>
+      <c r="F5" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,F$2)</f>
-        <v>121.38</v>
-      </c>
-      <c r="G5" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G5" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,G$2)</f>
-        <v>43249.921901111113</v>
-      </c>
-      <c r="H5" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H5" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B5,H$2)</f>
-        <v>43249.921901145834</v>
-      </c>
-      <c r="I5" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I5" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>2.9998831450939178</v>
-      </c>
-      <c r="J5" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" s="9" t="e">
         <f t="shared" si="0"/>
-        <v>4.9055555427912623E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K5" s="4">
         <f>RTD("rabbit",,"localhost",$K$1,$B5,K$2)</f>
-        <v>121.47</v>
+        <v>116.76</v>
       </c>
       <c r="L5" s="6">
         <f>RTD("rabbit",,"localhost",$K$1,$B5,L$2)</f>
-        <v>43249.921999189814</v>
+        <v>43250.778610671296</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -1297,35 +1433,35 @@
       </c>
       <c r="C6" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,C$2)</f>
-        <v>4.1359999999999999E-3</v>
+        <v>4.0800000000000003E-3</v>
       </c>
       <c r="D6" s="12">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,D$2)</f>
-        <v>4.1549999999999998E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="E6" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B6,E$2)</f>
-        <v>43249.921987037036</v>
-      </c>
-      <c r="F6" s="3">
+        <v>43250.778602685183</v>
+      </c>
+      <c r="F6" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,F$2)</f>
-        <v>4.1460000000000004E-3</v>
-      </c>
-      <c r="G6" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G6" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,G$2)</f>
-        <v>43249.921901377318</v>
-      </c>
-      <c r="H6" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H6" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B6,H$2)</f>
-        <v>43249.921900162037</v>
-      </c>
-      <c r="I6" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I6" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>-105.00031057745218</v>
-      </c>
-      <c r="J6" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="9" t="e">
         <f t="shared" si="0"/>
-        <v>4.902893488178961E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K6" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$K$1,$B6,K$2)</f>
@@ -1342,35 +1478,35 @@
       </c>
       <c r="C7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,C$2)</f>
-        <v>7.7188000000000007E-2</v>
+        <v>7.5005000000000002E-2</v>
       </c>
       <c r="D7">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,D$2)</f>
-        <v>7.7248999999999998E-2</v>
+        <v>7.5059000000000001E-2</v>
       </c>
       <c r="E7" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B7,E$2)</f>
-        <v>43249.921997523146</v>
-      </c>
-      <c r="F7" s="3">
+        <v>43250.778605717591</v>
+      </c>
+      <c r="F7" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,F$2)</f>
-        <v>7.7218999999999996E-2</v>
-      </c>
-      <c r="G7" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G7" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,G$2)</f>
-        <v>43249.921900787034</v>
-      </c>
-      <c r="H7" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H7" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B7,H$2)</f>
-        <v>43249.921904606483</v>
-      </c>
-      <c r="I7" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I7" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>330.00034745782614</v>
-      </c>
-      <c r="J7" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J7" s="9" t="e">
         <f t="shared" si="0"/>
-        <v>4.9087963270721957E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K7" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$K$1,$B7,K$2)</f>
@@ -1387,35 +1523,35 @@
       </c>
       <c r="C8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,C$2)</f>
-        <v>1.6136000000000001E-2</v>
+        <v>1.5890000000000001E-2</v>
       </c>
       <c r="D8">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,D$2)</f>
-        <v>1.6140000000000002E-2</v>
+        <v>1.5890999999999999E-2</v>
       </c>
       <c r="E8" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B8,E$2)</f>
-        <v>43249.921970763891</v>
-      </c>
-      <c r="F8" s="3">
+        <v>43250.778599166668</v>
+      </c>
+      <c r="F8" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,F$2)</f>
-        <v>1.6138E-2</v>
-      </c>
-      <c r="G8" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G8" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,G$2)</f>
-        <v>43249.921888935183</v>
-      </c>
-      <c r="H8" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H8" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B8,H$2)</f>
-        <v>43249.921887187498</v>
-      </c>
-      <c r="I8" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I8" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>-150.99998563528061</v>
-      </c>
-      <c r="J8" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="9" t="e">
         <f t="shared" si="0"/>
-        <v>5.0273148372070864E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K8" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$K$1,$B8,K$2)</f>
@@ -1432,35 +1568,35 @@
       </c>
       <c r="C9">
         <f>RTD("rabbit",,"localhost","BINANCE",$B9,C$2)</f>
-        <v>12.712</v>
+        <v>12.371600000000001</v>
       </c>
       <c r="D9">
         <f>RTD("rabbit",,"localhost","BINANCE",$B9,D$2)</f>
-        <v>12.729900000000001</v>
+        <v>12.39</v>
       </c>
       <c r="E9" s="5">
         <f>RTD("rabbit",,"localhost","BINANCE",$B9,E$2)</f>
-        <v>43249.92199091435</v>
-      </c>
-      <c r="F9" s="3">
+        <v>43250.778593726849</v>
+      </c>
+      <c r="F9" s="3" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B9,F$2)</f>
-        <v>12.72085</v>
-      </c>
-      <c r="G9" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="G9" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B9,G$2)</f>
-        <v>43249.921889131947</v>
-      </c>
-      <c r="H9" s="11">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="H9" s="11" t="str">
         <f>RTD("rabbit",,"localhost","MODEL",$B9,H$2)</f>
-        <v>43249.92188681713</v>
-      </c>
-      <c r="I9" s="7">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I9" s="7" t="e">
         <f t="shared" ref="I9" si="2">(H9-G9)*86400000</f>
-        <v>-200.00017248094082</v>
-      </c>
-      <c r="J9" s="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" s="9" t="e">
         <f t="shared" ref="J9" si="3">(CLOCK-G9)</f>
-        <v>5.0253471999894828E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K9" s="4" t="str">
         <f>RTD("rabbit",,"localhost",$K$1,$B9,K$2)</f>
@@ -1472,15 +1608,106 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J13" s="10">
-        <f>MIN(J3:J8)</f>
-        <v>4.902893488178961E-4</v>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="str">
+        <f>RTD("rabbit",,"MODEL",$B14,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D14" t="str">
+        <f>RTD("rabbit",,"MODEL",$B14,D$13)</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f>C3*0.001</f>
-        <v>7.523600000000001</v>
+      <c r="B15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="str">
+        <f>RTD("rabbit",,"MODEL",$B15,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D15" t="str">
+        <f>RTD("rabbit",,"MODEL",$B15,D$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="str">
+        <f>RTD("rabbit",,"MODEL",$B16,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D16" t="str">
+        <f>RTD("rabbit",,"MODEL",$B16,D$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RTD("rabbit",,"MODEL",$B17,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D17" t="str">
+        <f>RTD("rabbit",,"MODEL",$B17,D$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="str">
+        <f>RTD("rabbit",,"MODEL",$B18,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D18" t="str">
+        <f>RTD("rabbit",,"MODEL",$B18,D$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="str">
+        <f>RTD("rabbit",,"MODEL",$B19,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D19" t="str">
+        <f>RTD("rabbit",,"MODEL",$B19,D$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="str">
+        <f>RTD("rabbit",,"MODEL",$B20,C$13)</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D20" t="str">
+        <f>RTD("rabbit",,"MODEL",$B20,D$13)</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>